<commit_message>
fix typo and improved the experiment instruction
</commit_message>
<xml_diff>
--- a/instructions/arguments.xlsx
+++ b/instructions/arguments.xlsx
@@ -24,10 +24,6 @@
     <t>show_missing_word</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Premete la barra spaziatrice per visualizzare il termine mancante.</t>
-  </si>
-  <si>
     <t>La conclusione segue dalla premesse?</t>
   </si>
   <si>
@@ -45,6 +41,10 @@
   </si>
   <si>
     <t>+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Premere la barra spaziatrice per visualizzare il termine mancante</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -438,27 +438,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="270">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>